<commit_message>
Bonus question and adjustments to 2g
</commit_message>
<xml_diff>
--- a/docs/assignment-2.xlsx
+++ b/docs/assignment-2.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ishan\source\Repos\finc-2339-real-estate-capital-markets\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99221F55-B12D-4A38-B928-5289665AC6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26DF483-DA9D-46B0-8468-449CBF3CFD1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="18648" windowHeight="11784" xr2:uid="{5186C481-172D-DD4F-ABA8-8ABAE4599024}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="18648" windowHeight="11784" activeTab="1" xr2:uid="{5186C481-172D-DD4F-ABA8-8ABAE4599024}"/>
   </bookViews>
   <sheets>
-    <sheet name="Questio 2" sheetId="3" r:id="rId1"/>
+    <sheet name="Question 2 Part C" sheetId="3" r:id="rId1"/>
+    <sheet name="Question 2 Part H" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
   <si>
     <t>SMM</t>
   </si>
@@ -116,9 +117,9 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0000%"/>
-    <numFmt numFmtId="167" formatCode="0.0%"/>
-    <numFmt numFmtId="172" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="173" formatCode="&quot;$&quot;#,##0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -233,7 +234,7 @@
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -247,8 +248,8 @@
     <xf numFmtId="43" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="4" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -591,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F604A89-6593-8043-BE2C-6F1D1402DDAF}">
   <dimension ref="A1:Q181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="102" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView zoomScale="102" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -762,7 +763,7 @@
         <v>1173975.1156675508</v>
       </c>
       <c r="J3" s="17">
-        <f t="shared" ref="J2:J33" si="3">$Q$2/12*B3</f>
+        <f t="shared" ref="J3:J33" si="3">$Q$2/12*B3</f>
         <v>1120238.3514016727</v>
       </c>
       <c r="K3" s="17">
@@ -10978,6 +10979,3614 @@
       <c r="N181" s="17">
         <f t="shared" si="34"/>
         <v>399047.88540127635</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEDD236B-69F1-4BAE-B5E0-A7D4B1088073}">
+  <dimension ref="A1:Q62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="J8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.296875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="16" style="18" customWidth="1"/>
+    <col min="3" max="3" width="14" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.09765625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.296875" style="12" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="12" customWidth="1"/>
+    <col min="7" max="7" width="15.3984375" style="18" customWidth="1"/>
+    <col min="8" max="8" width="16" style="18" customWidth="1"/>
+    <col min="9" max="9" width="14.3984375" style="18" customWidth="1"/>
+    <col min="10" max="10" width="12.59765625" style="18" customWidth="1"/>
+    <col min="11" max="11" width="13.796875" style="18" customWidth="1"/>
+    <col min="12" max="12" width="14.3984375" style="18" customWidth="1"/>
+    <col min="13" max="13" width="12.3984375" style="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.8984375" style="18" customWidth="1"/>
+    <col min="15" max="15" width="11.19921875" style="12"/>
+    <col min="16" max="16" width="25.3984375" style="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.296875" style="12" customWidth="1"/>
+    <col min="18" max="16384" width="11.19921875" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="7" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="6"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17">
+        <f>Q6</f>
+        <v>300000000</v>
+      </c>
+      <c r="C2" s="9">
+        <f>(0.2*A2*1)/100</f>
+        <v>2E-3</v>
+      </c>
+      <c r="D2" s="9">
+        <f>C2*2</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E2" s="10">
+        <f>1-(1-D2)^(1/12)</f>
+        <v>3.3394601074221431E-4</v>
+      </c>
+      <c r="F2" s="11">
+        <f>1-E2</f>
+        <v>0.99966605398925779</v>
+      </c>
+      <c r="G2" s="17">
+        <f>PMT(Q2/12,12*$Q$3,-Q6)</f>
+        <v>2294979.8664403548</v>
+      </c>
+      <c r="H2" s="17">
+        <f>B2-I2</f>
+        <v>298830020.13355964</v>
+      </c>
+      <c r="I2" s="17">
+        <f>G2-J2</f>
+        <v>1169979.8664403548</v>
+      </c>
+      <c r="J2" s="17">
+        <f>$Q$2/12*B2</f>
+        <v>1125000</v>
+      </c>
+      <c r="K2" s="17">
+        <f>H2*E2</f>
+        <v>99793.093113617826</v>
+      </c>
+      <c r="L2" s="17">
+        <f>SUM(I2:K2)</f>
+        <v>2394772.9595539728</v>
+      </c>
+      <c r="M2" s="17">
+        <f>$Q$4*B2/(100*100*12)</f>
+        <v>125000</v>
+      </c>
+      <c r="N2" s="17">
+        <f>L2-M2</f>
+        <v>2269772.9595539728</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="13">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17">
+        <f>B2-I2-K2</f>
+        <v>298730227.04044604</v>
+      </c>
+      <c r="C3" s="9">
+        <f t="shared" ref="C3:C31" si="0">(0.2*A3*1)/100</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D3" s="9">
+        <f t="shared" ref="D3:D62" si="1">C3*2</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E3" s="10">
+        <f t="shared" ref="E3:E62" si="2">1-(1-D3)^(1/12)</f>
+        <v>6.6912367827864916E-4</v>
+      </c>
+      <c r="F3" s="11">
+        <f>F2*(1-E3)</f>
+        <v>0.99899715376216214</v>
+      </c>
+      <c r="G3" s="17">
+        <f>$G$2*F2</f>
+        <v>2294213.4670692235</v>
+      </c>
+      <c r="H3" s="17">
+        <f>B3-I3</f>
+        <v>297556251.92477852</v>
+      </c>
+      <c r="I3" s="17">
+        <f>G3-J3</f>
+        <v>1173975.1156675508</v>
+      </c>
+      <c r="J3" s="17">
+        <f t="shared" ref="J3:J62" si="3">$Q$2/12*B3</f>
+        <v>1120238.3514016727</v>
+      </c>
+      <c r="K3" s="17">
+        <f>H3*E3</f>
+        <v>199101.93378271619</v>
+      </c>
+      <c r="L3" s="17">
+        <f t="shared" ref="L3:L62" si="4">SUM(I3:K3)</f>
+        <v>2493315.4008519398</v>
+      </c>
+      <c r="M3" s="17">
+        <f t="shared" ref="M3:M62" si="5">$Q$4*B3/(100*100*12)</f>
+        <v>124470.92793351918</v>
+      </c>
+      <c r="N3" s="17">
+        <f t="shared" ref="N3:N62" si="6">L3-M3</f>
+        <v>2368844.4729184206</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q3" s="21">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17">
+        <f t="shared" ref="B4:B62" si="7">B3-I3-K3</f>
+        <v>297357149.99099582</v>
+      </c>
+      <c r="C4" s="9">
+        <f t="shared" si="0"/>
+        <v>6.000000000000001E-3</v>
+      </c>
+      <c r="D4" s="9">
+        <f t="shared" si="1"/>
+        <v>1.2000000000000002E-2</v>
+      </c>
+      <c r="E4" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0055425391276573E-3</v>
+      </c>
+      <c r="F4" s="11">
+        <f t="shared" ref="F4:F62" si="8">F3*(1-E4)</f>
+        <v>0.99799261962758679</v>
+      </c>
+      <c r="G4" s="17">
+        <f t="shared" ref="G4:G62" si="9">$G$2*F3</f>
+        <v>2292678.3545153816</v>
+      </c>
+      <c r="H4" s="17">
+        <f t="shared" ref="H4:H62" si="10">B4-I4</f>
+        <v>296179560.94894665</v>
+      </c>
+      <c r="I4" s="17">
+        <f>G4-J4</f>
+        <v>1177589.0420491474</v>
+      </c>
+      <c r="J4" s="17">
+        <f t="shared" si="3"/>
+        <v>1115089.3124662342</v>
+      </c>
+      <c r="K4" s="17">
+        <f t="shared" ref="K4:K62" si="11">H4*E4</f>
+        <v>297821.14775431855</v>
+      </c>
+      <c r="L4" s="17">
+        <f t="shared" si="4"/>
+        <v>2590499.5022697002</v>
+      </c>
+      <c r="M4" s="17">
+        <f t="shared" si="5"/>
+        <v>123898.81249624825</v>
+      </c>
+      <c r="N4" s="17">
+        <f t="shared" si="6"/>
+        <v>2466600.689773452</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="17">
+        <f t="shared" si="7"/>
+        <v>295881739.80119234</v>
+      </c>
+      <c r="C5" s="9">
+        <f t="shared" si="0"/>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D5" s="9">
+        <f t="shared" si="1"/>
+        <v>1.6E-2</v>
+      </c>
+      <c r="E5" s="10">
+        <f t="shared" si="2"/>
+        <v>1.3432122426282334E-3</v>
+      </c>
+      <c r="F5" s="11">
+        <f t="shared" si="8"/>
+        <v>0.9966521037228504</v>
+      </c>
+      <c r="G5" s="17">
+        <f t="shared" si="9"/>
+        <v>2290372.968901379</v>
+      </c>
+      <c r="H5" s="17">
+        <f t="shared" si="10"/>
+        <v>294700923.35654545</v>
+      </c>
+      <c r="I5" s="17">
+        <f t="shared" ref="I5:I62" si="12">G5-J5</f>
+        <v>1180816.4446469077</v>
+      </c>
+      <c r="J5" s="17">
+        <f t="shared" si="3"/>
+        <v>1109556.5242544713</v>
+      </c>
+      <c r="K5" s="17">
+        <f t="shared" si="11"/>
+        <v>395845.88816635654</v>
+      </c>
+      <c r="L5" s="17">
+        <f t="shared" si="4"/>
+        <v>2686218.8570677354</v>
+      </c>
+      <c r="M5" s="17">
+        <f t="shared" si="5"/>
+        <v>123284.05825049682</v>
+      </c>
+      <c r="N5" s="17">
+        <f t="shared" si="6"/>
+        <v>2562934.7988172388</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q5" s="12">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="17">
+        <f t="shared" si="7"/>
+        <v>294305077.46837908</v>
+      </c>
+      <c r="C6" s="9">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="D6" s="9">
+        <f t="shared" si="1"/>
+        <v>0.02</v>
+      </c>
+      <c r="E6" s="10">
+        <f t="shared" si="2"/>
+        <v>1.6821425527395739E-3</v>
+      </c>
+      <c r="F6" s="11">
+        <f t="shared" si="8"/>
+        <v>0.9949755928089008</v>
+      </c>
+      <c r="G6" s="17">
+        <f t="shared" si="9"/>
+        <v>2287296.511889366</v>
+      </c>
+      <c r="H6" s="17">
+        <f t="shared" si="10"/>
+        <v>293121424.99699616</v>
+      </c>
+      <c r="I6" s="17">
+        <f t="shared" si="12"/>
+        <v>1183652.4713829444</v>
+      </c>
+      <c r="J6" s="17">
+        <f t="shared" si="3"/>
+        <v>1103644.0405064216</v>
+      </c>
+      <c r="K6" s="17">
+        <f t="shared" si="11"/>
+        <v>493072.02210710867</v>
+      </c>
+      <c r="L6" s="17">
+        <f t="shared" si="4"/>
+        <v>2780368.5339964745</v>
+      </c>
+      <c r="M6" s="17">
+        <f t="shared" si="5"/>
+        <v>122627.11561182463</v>
+      </c>
+      <c r="N6" s="17">
+        <f t="shared" si="6"/>
+        <v>2657741.4183846498</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q6" s="14">
+        <v>300000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
+        <v>6</v>
+      </c>
+      <c r="B7" s="17">
+        <f t="shared" si="7"/>
+        <v>292628352.97488904</v>
+      </c>
+      <c r="C7" s="9">
+        <f t="shared" si="0"/>
+        <v>1.2000000000000002E-2</v>
+      </c>
+      <c r="D7" s="9">
+        <f t="shared" si="1"/>
+        <v>2.4000000000000004E-2</v>
+      </c>
+      <c r="E7" s="10">
+        <f t="shared" si="2"/>
+        <v>2.0223433498771648E-3</v>
+      </c>
+      <c r="F7" s="11">
+        <f t="shared" si="8"/>
+        <v>0.99296341053549364</v>
+      </c>
+      <c r="G7" s="17">
+        <f t="shared" si="9"/>
+        <v>2283448.9530959842</v>
+      </c>
+      <c r="H7" s="17">
+        <f t="shared" si="10"/>
+        <v>291442260.34544891</v>
+      </c>
+      <c r="I7" s="17">
+        <f t="shared" si="12"/>
+        <v>1186092.6294401502</v>
+      </c>
+      <c r="J7" s="17">
+        <f t="shared" si="3"/>
+        <v>1097356.323655834</v>
+      </c>
+      <c r="K7" s="17">
+        <f t="shared" si="11"/>
+        <v>589396.31708278798</v>
+      </c>
+      <c r="L7" s="17">
+        <f t="shared" si="4"/>
+        <v>2872845.270178772</v>
+      </c>
+      <c r="M7" s="17">
+        <f t="shared" si="5"/>
+        <v>121928.48040620376</v>
+      </c>
+      <c r="N7" s="17">
+        <f t="shared" si="6"/>
+        <v>2750916.7897725683</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="17">
+        <f t="shared" si="7"/>
+        <v>290852864.02836615</v>
+      </c>
+      <c r="C8" s="9">
+        <f t="shared" si="0"/>
+        <v>1.4000000000000002E-2</v>
+      </c>
+      <c r="D8" s="9">
+        <f t="shared" si="1"/>
+        <v>2.8000000000000004E-2</v>
+      </c>
+      <c r="E8" s="10">
+        <f t="shared" si="2"/>
+        <v>2.3638246327857271E-3</v>
+      </c>
+      <c r="F8" s="11">
+        <f t="shared" si="8"/>
+        <v>0.9906162191662149</v>
+      </c>
+      <c r="G8" s="17">
+        <f t="shared" si="9"/>
+        <v>2278831.0352909062</v>
+      </c>
+      <c r="H8" s="17">
+        <f t="shared" si="10"/>
+        <v>289664731.2331816</v>
+      </c>
+      <c r="I8" s="17">
+        <f t="shared" si="12"/>
+        <v>1188132.7951845331</v>
+      </c>
+      <c r="J8" s="17">
+        <f t="shared" si="3"/>
+        <v>1090698.2401063731</v>
+      </c>
+      <c r="K8" s="17">
+        <f t="shared" si="11"/>
+        <v>684716.62693825178</v>
+      </c>
+      <c r="L8" s="17">
+        <f t="shared" si="4"/>
+        <v>2963547.662229158</v>
+      </c>
+      <c r="M8" s="17">
+        <f t="shared" si="5"/>
+        <v>121188.69334515257</v>
+      </c>
+      <c r="N8" s="17">
+        <f t="shared" si="6"/>
+        <v>2842358.9688840052</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q8" s="24">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
+        <v>8</v>
+      </c>
+      <c r="B9" s="17">
+        <f t="shared" si="7"/>
+        <v>288980014.60624337</v>
+      </c>
+      <c r="C9" s="9">
+        <f t="shared" si="0"/>
+        <v>1.6E-2</v>
+      </c>
+      <c r="D9" s="9">
+        <f t="shared" si="1"/>
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="E9" s="10">
+        <f t="shared" si="2"/>
+        <v>2.7065965204493558E-3</v>
+      </c>
+      <c r="F9" s="11">
+        <f t="shared" si="8"/>
+        <v>0.98793502075431894</v>
+      </c>
+      <c r="G9" s="17">
+        <f t="shared" si="9"/>
+        <v>2273444.2783557293</v>
+      </c>
+      <c r="H9" s="17">
+        <f t="shared" si="10"/>
+        <v>287790245.38266104</v>
+      </c>
+      <c r="I9" s="17">
+        <f t="shared" si="12"/>
+        <v>1189769.2235823167</v>
+      </c>
+      <c r="J9" s="17">
+        <f t="shared" si="3"/>
+        <v>1083675.0547734126</v>
+      </c>
+      <c r="K9" s="17">
+        <f t="shared" si="11"/>
+        <v>778932.07677197666</v>
+      </c>
+      <c r="L9" s="17">
+        <f t="shared" si="4"/>
+        <v>3052376.3551277062</v>
+      </c>
+      <c r="M9" s="17">
+        <f t="shared" si="5"/>
+        <v>120408.33941926807</v>
+      </c>
+      <c r="N9" s="17">
+        <f t="shared" si="6"/>
+        <v>2931968.0157084381</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q9" s="15">
+        <f>NPV($Q$8/12,M2:M61)</f>
+        <v>5024867.7428505374</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
+        <v>9</v>
+      </c>
+      <c r="B10" s="17">
+        <f t="shared" si="7"/>
+        <v>287011313.30588907</v>
+      </c>
+      <c r="C10" s="9">
+        <f t="shared" si="0"/>
+        <v>1.8000000000000002E-2</v>
+      </c>
+      <c r="D10" s="9">
+        <f t="shared" si="1"/>
+        <v>3.6000000000000004E-2</v>
+      </c>
+      <c r="E10" s="10">
+        <f t="shared" si="2"/>
+        <v>3.0506692540422931E-3</v>
+      </c>
+      <c r="F10" s="11">
+        <f t="shared" si="8"/>
+        <v>0.98492115776151212</v>
+      </c>
+      <c r="G10" s="17">
+        <f t="shared" si="9"/>
+        <v>2267290.9819824961</v>
+      </c>
+      <c r="H10" s="17">
+        <f t="shared" si="10"/>
+        <v>285820314.74880368</v>
+      </c>
+      <c r="I10" s="17">
+        <f t="shared" si="12"/>
+        <v>1190998.5570854121</v>
+      </c>
+      <c r="J10" s="17">
+        <f t="shared" si="3"/>
+        <v>1076292.424897084</v>
+      </c>
+      <c r="K10" s="17">
+        <f t="shared" si="11"/>
+        <v>871943.2463848663</v>
+      </c>
+      <c r="L10" s="17">
+        <f t="shared" si="4"/>
+        <v>3139234.2283673622</v>
+      </c>
+      <c r="M10" s="17">
+        <f t="shared" si="5"/>
+        <v>119588.0472107871</v>
+      </c>
+      <c r="N10" s="17">
+        <f t="shared" si="6"/>
+        <v>3019646.1811565752</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q10" s="15">
+        <f>NPV($Q$8/12,N2:N61)</f>
+        <v>289950264.51429927</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
+        <v>10</v>
+      </c>
+      <c r="B11" s="17">
+        <f t="shared" si="7"/>
+        <v>284948371.50241882</v>
+      </c>
+      <c r="C11" s="9">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="D11" s="9">
+        <f t="shared" si="1"/>
+        <v>0.04</v>
+      </c>
+      <c r="E11" s="10">
+        <f t="shared" si="2"/>
+        <v>3.3960531989175591E-3</v>
+      </c>
+      <c r="F11" s="11">
+        <f t="shared" si="8"/>
+        <v>0.98157631311301452</v>
+      </c>
+      <c r="G11" s="17">
+        <f t="shared" si="9"/>
+        <v>2260374.2270937948</v>
+      </c>
+      <c r="H11" s="17">
+        <f t="shared" si="10"/>
+        <v>283756553.66845912</v>
+      </c>
+      <c r="I11" s="17">
+        <f t="shared" si="12"/>
+        <v>1191817.8339597243</v>
+      </c>
+      <c r="J11" s="17">
+        <f t="shared" si="3"/>
+        <v>1068556.3931340706</v>
+      </c>
+      <c r="K11" s="17">
+        <f t="shared" si="11"/>
+        <v>963652.35179959261</v>
+      </c>
+      <c r="L11" s="17">
+        <f t="shared" si="4"/>
+        <v>3224026.5788933877</v>
+      </c>
+      <c r="M11" s="17">
+        <f t="shared" si="5"/>
+        <v>118728.48812600784</v>
+      </c>
+      <c r="N11" s="17">
+        <f t="shared" si="6"/>
+        <v>3105298.0907673799</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q11" s="15">
+        <f>NPV($Q$8/12,L2:L61)</f>
+        <v>294975132.25714976</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="8">
+        <v>11</v>
+      </c>
+      <c r="B12" s="17">
+        <f t="shared" si="7"/>
+        <v>282792901.31665951</v>
+      </c>
+      <c r="C12" s="9">
+        <f t="shared" si="0"/>
+        <v>2.2000000000000002E-2</v>
+      </c>
+      <c r="D12" s="9">
+        <f t="shared" si="1"/>
+        <v>4.4000000000000004E-2</v>
+      </c>
+      <c r="E12" s="10">
+        <f t="shared" si="2"/>
+        <v>3.7427588466381057E-3</v>
+      </c>
+      <c r="F12" s="11">
+        <f t="shared" si="8"/>
+        <v>0.97790250968346037</v>
+      </c>
+      <c r="G12" s="17">
+        <f t="shared" si="9"/>
+        <v>2252697.8759691222</v>
+      </c>
+      <c r="H12" s="17">
+        <f t="shared" si="10"/>
+        <v>281600676.82062787</v>
+      </c>
+      <c r="I12" s="17">
+        <f t="shared" si="12"/>
+        <v>1192224.4960316489</v>
+      </c>
+      <c r="J12" s="17">
+        <f t="shared" si="3"/>
+        <v>1060473.3799374732</v>
+      </c>
+      <c r="K12" s="17">
+        <f t="shared" si="11"/>
+        <v>1053963.4243896832</v>
+      </c>
+      <c r="L12" s="17">
+        <f t="shared" si="4"/>
+        <v>3306661.3003588053</v>
+      </c>
+      <c r="M12" s="17">
+        <f t="shared" si="5"/>
+        <v>117830.37554860814</v>
+      </c>
+      <c r="N12" s="17">
+        <f t="shared" si="6"/>
+        <v>3188830.9248101972</v>
+      </c>
+      <c r="Q12" s="22"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="8">
+        <v>12</v>
+      </c>
+      <c r="B13" s="17">
+        <f t="shared" si="7"/>
+        <v>280546713.39623821</v>
+      </c>
+      <c r="C13" s="9">
+        <f t="shared" si="0"/>
+        <v>2.4000000000000004E-2</v>
+      </c>
+      <c r="D13" s="9">
+        <f t="shared" si="1"/>
+        <v>4.8000000000000008E-2</v>
+      </c>
+      <c r="E13" s="10">
+        <f t="shared" si="2"/>
+        <v>4.0907968170484921E-3</v>
+      </c>
+      <c r="F13" s="11">
+        <f t="shared" si="8"/>
+        <v>0.97390210920946352</v>
+      </c>
+      <c r="G13" s="17">
+        <f t="shared" si="9"/>
+        <v>2244266.5710650356</v>
+      </c>
+      <c r="H13" s="17">
+        <f t="shared" si="10"/>
+        <v>279354497.00040907</v>
+      </c>
+      <c r="I13" s="17">
+        <f t="shared" si="12"/>
+        <v>1192216.3958291423</v>
+      </c>
+      <c r="J13" s="17">
+        <f t="shared" si="3"/>
+        <v>1052050.1752358933</v>
+      </c>
+      <c r="K13" s="17">
+        <f t="shared" si="11"/>
+        <v>1142782.4871574559</v>
+      </c>
+      <c r="L13" s="17">
+        <f t="shared" si="4"/>
+        <v>3387049.0582224913</v>
+      </c>
+      <c r="M13" s="17">
+        <f t="shared" si="5"/>
+        <v>116894.46391509926</v>
+      </c>
+      <c r="N13" s="17">
+        <f t="shared" si="6"/>
+        <v>3270154.5943073919</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="8">
+        <v>13</v>
+      </c>
+      <c r="B14" s="17">
+        <f t="shared" si="7"/>
+        <v>278211714.5132516</v>
+      </c>
+      <c r="C14" s="9">
+        <f t="shared" si="0"/>
+        <v>2.6000000000000002E-2</v>
+      </c>
+      <c r="D14" s="9">
+        <f t="shared" si="1"/>
+        <v>5.2000000000000005E-2</v>
+      </c>
+      <c r="E14" s="10">
+        <f t="shared" si="2"/>
+        <v>4.4401778603907482E-3</v>
+      </c>
+      <c r="F14" s="11">
+        <f t="shared" si="8"/>
+        <v>0.96957781062596382</v>
+      </c>
+      <c r="G14" s="17">
+        <f t="shared" si="9"/>
+        <v>2235085.7325195144</v>
+      </c>
+      <c r="H14" s="17">
+        <f t="shared" si="10"/>
+        <v>277019922.7101568</v>
+      </c>
+      <c r="I14" s="17">
+        <f t="shared" si="12"/>
+        <v>1191791.8030948211</v>
+      </c>
+      <c r="J14" s="17">
+        <f t="shared" si="3"/>
+        <v>1043293.9294246935</v>
+      </c>
+      <c r="K14" s="17">
+        <f t="shared" si="11"/>
+        <v>1230017.7277047944</v>
+      </c>
+      <c r="L14" s="17">
+        <f t="shared" si="4"/>
+        <v>3465103.460224309</v>
+      </c>
+      <c r="M14" s="17">
+        <f t="shared" si="5"/>
+        <v>115921.54771385483</v>
+      </c>
+      <c r="N14" s="17">
+        <f t="shared" si="6"/>
+        <v>3349181.9125104542</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="8">
+        <v>14</v>
+      </c>
+      <c r="B15" s="17">
+        <f t="shared" si="7"/>
+        <v>275789904.98245198</v>
+      </c>
+      <c r="C15" s="9">
+        <f t="shared" si="0"/>
+        <v>2.8000000000000004E-2</v>
+      </c>
+      <c r="D15" s="9">
+        <f t="shared" si="1"/>
+        <v>5.6000000000000008E-2</v>
+      </c>
+      <c r="E15" s="10">
+        <f t="shared" si="2"/>
+        <v>4.7909128594627592E-3</v>
+      </c>
+      <c r="F15" s="11">
+        <f t="shared" si="8"/>
+        <v>0.96493264782478616</v>
+      </c>
+      <c r="G15" s="17">
+        <f t="shared" si="9"/>
+        <v>2225161.5543339062</v>
+      </c>
+      <c r="H15" s="17">
+        <f t="shared" si="10"/>
+        <v>274598955.57180226</v>
+      </c>
+      <c r="I15" s="17">
+        <f t="shared" si="12"/>
+        <v>1190949.4106497113</v>
+      </c>
+      <c r="J15" s="17">
+        <f t="shared" si="3"/>
+        <v>1034212.1436841949</v>
+      </c>
+      <c r="K15" s="17">
+        <f t="shared" si="11"/>
+        <v>1315579.6674439902</v>
+      </c>
+      <c r="L15" s="17">
+        <f t="shared" si="4"/>
+        <v>3540741.2217778964</v>
+      </c>
+      <c r="M15" s="17">
+        <f t="shared" si="5"/>
+        <v>114912.46040935499</v>
+      </c>
+      <c r="N15" s="17">
+        <f t="shared" si="6"/>
+        <v>3425828.7613685415</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="8">
+        <v>15</v>
+      </c>
+      <c r="B16" s="17">
+        <f t="shared" si="7"/>
+        <v>273283375.90435827</v>
+      </c>
+      <c r="C16" s="9">
+        <f t="shared" si="0"/>
+        <v>0.03</v>
+      </c>
+      <c r="D16" s="9">
+        <f t="shared" si="1"/>
+        <v>0.06</v>
+      </c>
+      <c r="E16" s="10">
+        <f t="shared" si="2"/>
+        <v>5.1430128318229462E-3</v>
+      </c>
+      <c r="F16" s="11">
+        <f t="shared" si="8"/>
+        <v>0.95996998683517842</v>
+      </c>
+      <c r="G16" s="17">
+        <f t="shared" si="9"/>
+        <v>2214500.9992288658</v>
+      </c>
+      <c r="H16" s="17">
+        <f t="shared" si="10"/>
+        <v>272093687.56477076</v>
+      </c>
+      <c r="I16" s="17">
+        <f t="shared" si="12"/>
+        <v>1189688.3395875222</v>
+      </c>
+      <c r="J16" s="17">
+        <f t="shared" si="3"/>
+        <v>1024812.6596413435</v>
+      </c>
+      <c r="K16" s="17">
+        <f t="shared" si="11"/>
+        <v>1399381.3266036396</v>
+      </c>
+      <c r="L16" s="17">
+        <f t="shared" si="4"/>
+        <v>3613882.3258325057</v>
+      </c>
+      <c r="M16" s="17">
+        <f t="shared" si="5"/>
+        <v>113868.07329348261</v>
+      </c>
+      <c r="N16" s="17">
+        <f t="shared" si="6"/>
+        <v>3500014.2525390233</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="8">
+        <v>16</v>
+      </c>
+      <c r="B17" s="17">
+        <f t="shared" si="7"/>
+        <v>270694306.23816711</v>
+      </c>
+      <c r="C17" s="9">
+        <f t="shared" si="0"/>
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="D17" s="9">
+        <f t="shared" si="1"/>
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="E17" s="10">
+        <f t="shared" si="2"/>
+        <v>5.4964889320406884E-3</v>
+      </c>
+      <c r="F17" s="11">
+        <f t="shared" si="8"/>
+        <v>0.95469352242744765</v>
+      </c>
+      <c r="G17" s="17">
+        <f t="shared" si="9"/>
+        <v>2203111.792173747</v>
+      </c>
+      <c r="H17" s="17">
+        <f t="shared" si="10"/>
+        <v>269506298.09438646</v>
+      </c>
+      <c r="I17" s="17">
+        <f t="shared" si="12"/>
+        <v>1188008.1437806203</v>
+      </c>
+      <c r="J17" s="17">
+        <f t="shared" si="3"/>
+        <v>1015103.6483931267</v>
+      </c>
+      <c r="K17" s="17">
+        <f t="shared" si="11"/>
+        <v>1481338.3845910537</v>
+      </c>
+      <c r="L17" s="17">
+        <f t="shared" si="4"/>
+        <v>3684450.1767648007</v>
+      </c>
+      <c r="M17" s="17">
+        <f t="shared" si="5"/>
+        <v>112789.29426590296</v>
+      </c>
+      <c r="N17" s="17">
+        <f t="shared" si="6"/>
+        <v>3571660.8824988976</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="8">
+        <v>17</v>
+      </c>
+      <c r="B18" s="17">
+        <f t="shared" si="7"/>
+        <v>268024959.70979542</v>
+      </c>
+      <c r="C18" s="9">
+        <f t="shared" si="0"/>
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="D18" s="9">
+        <f t="shared" si="1"/>
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="E18" s="10">
+        <f t="shared" si="2"/>
+        <v>5.8513524539940409E-3</v>
+      </c>
+      <c r="F18" s="11">
+        <f t="shared" si="8"/>
+        <v>0.94910727414217955</v>
+      </c>
+      <c r="G18" s="17">
+        <f t="shared" si="9"/>
+        <v>2191002.4125920157</v>
+      </c>
+      <c r="H18" s="17">
+        <f t="shared" si="10"/>
+        <v>266839050.89611512</v>
+      </c>
+      <c r="I18" s="17">
+        <f t="shared" si="12"/>
+        <v>1185908.8136802828</v>
+      </c>
+      <c r="J18" s="17">
+        <f t="shared" si="3"/>
+        <v>1005093.5989117328</v>
+      </c>
+      <c r="K18" s="17">
+        <f t="shared" si="11"/>
+        <v>1561369.335282424</v>
+      </c>
+      <c r="L18" s="17">
+        <f t="shared" si="4"/>
+        <v>3752371.7478744397</v>
+      </c>
+      <c r="M18" s="17">
+        <f t="shared" si="5"/>
+        <v>111677.06654574809</v>
+      </c>
+      <c r="N18" s="17">
+        <f t="shared" si="6"/>
+        <v>3640694.6813286915</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="8">
+        <v>18</v>
+      </c>
+      <c r="B19" s="17">
+        <f t="shared" si="7"/>
+        <v>265277681.56083271</v>
+      </c>
+      <c r="C19" s="9">
+        <f t="shared" si="0"/>
+        <v>3.6000000000000004E-2</v>
+      </c>
+      <c r="D19" s="9">
+        <f t="shared" si="1"/>
+        <v>7.2000000000000008E-2</v>
+      </c>
+      <c r="E19" s="10">
+        <f t="shared" si="2"/>
+        <v>6.2076148332157466E-3</v>
+      </c>
+      <c r="F19" s="11">
+        <f t="shared" si="8"/>
+        <v>0.94321558174890163</v>
+      </c>
+      <c r="G19" s="17">
+        <f t="shared" si="9"/>
+        <v>2178182.0852483884</v>
+      </c>
+      <c r="H19" s="17">
+        <f t="shared" si="10"/>
+        <v>264094290.78143746</v>
+      </c>
+      <c r="I19" s="17">
+        <f t="shared" si="12"/>
+        <v>1183390.7793952657</v>
+      </c>
+      <c r="J19" s="17">
+        <f t="shared" si="3"/>
+        <v>994791.30585312261</v>
+      </c>
+      <c r="K19" s="17">
+        <f t="shared" si="11"/>
+        <v>1639395.6368224437</v>
+      </c>
+      <c r="L19" s="17">
+        <f t="shared" si="4"/>
+        <v>3817577.7220708318</v>
+      </c>
+      <c r="M19" s="17">
+        <f t="shared" si="5"/>
+        <v>110532.36731701363</v>
+      </c>
+      <c r="N19" s="17">
+        <f t="shared" si="6"/>
+        <v>3707045.3547538184</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="8">
+        <v>19</v>
+      </c>
+      <c r="B20" s="17">
+        <f t="shared" si="7"/>
+        <v>262454895.14461502</v>
+      </c>
+      <c r="C20" s="9">
+        <f t="shared" si="0"/>
+        <v>3.8000000000000006E-2</v>
+      </c>
+      <c r="D20" s="9">
+        <f t="shared" si="1"/>
+        <v>7.6000000000000012E-2</v>
+      </c>
+      <c r="E20" s="10">
+        <f t="shared" si="2"/>
+        <v>6.5652876492899859E-3</v>
+      </c>
+      <c r="F20" s="11">
+        <f t="shared" si="8"/>
+        <v>0.93702310013942769</v>
+      </c>
+      <c r="G20" s="17">
+        <f t="shared" si="9"/>
+        <v>2164660.7698265561</v>
+      </c>
+      <c r="H20" s="17">
+        <f t="shared" si="10"/>
+        <v>261274440.23158076</v>
+      </c>
+      <c r="I20" s="17">
+        <f t="shared" si="12"/>
+        <v>1180454.9130342498</v>
+      </c>
+      <c r="J20" s="17">
+        <f t="shared" si="3"/>
+        <v>984205.85679230629</v>
+      </c>
+      <c r="K20" s="17">
+        <f t="shared" si="11"/>
+        <v>1715341.8555275518</v>
+      </c>
+      <c r="L20" s="17">
+        <f t="shared" si="4"/>
+        <v>3880002.6253541079</v>
+      </c>
+      <c r="M20" s="17">
+        <f t="shared" si="5"/>
+        <v>109356.20631025625</v>
+      </c>
+      <c r="N20" s="17">
+        <f t="shared" si="6"/>
+        <v>3770646.4190438516</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="8">
+        <v>20</v>
+      </c>
+      <c r="B21" s="17">
+        <f t="shared" si="7"/>
+        <v>259559098.37605321</v>
+      </c>
+      <c r="C21" s="9">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="D21" s="9">
+        <f t="shared" si="1"/>
+        <v>0.08</v>
+      </c>
+      <c r="E21" s="10">
+        <f t="shared" si="2"/>
+        <v>6.9243826282994192E-3</v>
+      </c>
+      <c r="F21" s="11">
+        <f t="shared" si="8"/>
+        <v>0.93053479366250702</v>
+      </c>
+      <c r="G21" s="17">
+        <f t="shared" si="9"/>
+        <v>2150449.149209511</v>
+      </c>
+      <c r="H21" s="17">
+        <f t="shared" si="10"/>
+        <v>258381995.84575391</v>
+      </c>
+      <c r="I21" s="17">
+        <f t="shared" si="12"/>
+        <v>1177102.5302993115</v>
+      </c>
+      <c r="J21" s="17">
+        <f t="shared" si="3"/>
+        <v>973346.6189101995</v>
+      </c>
+      <c r="K21" s="17">
+        <f t="shared" si="11"/>
+        <v>1789135.8034996712</v>
+      </c>
+      <c r="L21" s="17">
+        <f t="shared" si="4"/>
+        <v>3939584.9527091822</v>
+      </c>
+      <c r="M21" s="17">
+        <f t="shared" si="5"/>
+        <v>108149.6243233555</v>
+      </c>
+      <c r="N21" s="17">
+        <f t="shared" si="6"/>
+        <v>3831435.3283858267</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="8">
+        <v>21</v>
+      </c>
+      <c r="B22" s="17">
+        <f t="shared" si="7"/>
+        <v>256592860.04225424</v>
+      </c>
+      <c r="C22" s="9">
+        <f t="shared" si="0"/>
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="D22" s="9">
+        <f t="shared" si="1"/>
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="E22" s="10">
+        <f t="shared" si="2"/>
+        <v>7.2849116453249652E-3</v>
+      </c>
+      <c r="F22" s="11">
+        <f t="shared" si="8"/>
+        <v>0.923755929907775</v>
+      </c>
+      <c r="G22" s="17">
+        <f t="shared" si="9"/>
+        <v>2135558.6164776837</v>
+      </c>
+      <c r="H22" s="17">
+        <f t="shared" si="10"/>
+        <v>255419524.65093499</v>
+      </c>
+      <c r="I22" s="17">
+        <f t="shared" si="12"/>
+        <v>1173335.3913192302</v>
+      </c>
+      <c r="J22" s="17">
+        <f t="shared" si="3"/>
+        <v>962223.22515845334</v>
+      </c>
+      <c r="K22" s="17">
+        <f t="shared" si="11"/>
+        <v>1860708.6695729634</v>
+      </c>
+      <c r="L22" s="17">
+        <f t="shared" si="4"/>
+        <v>3996267.286050647</v>
+      </c>
+      <c r="M22" s="17">
+        <f t="shared" si="5"/>
+        <v>106913.69168427261</v>
+      </c>
+      <c r="N22" s="17">
+        <f t="shared" si="6"/>
+        <v>3889353.5943663744</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" s="8">
+        <v>22</v>
+      </c>
+      <c r="B23" s="17">
+        <f t="shared" si="7"/>
+        <v>253558815.98136204</v>
+      </c>
+      <c r="C23" s="9">
+        <f t="shared" si="0"/>
+        <v>4.4000000000000004E-2</v>
+      </c>
+      <c r="D23" s="9">
+        <f t="shared" si="1"/>
+        <v>8.8000000000000009E-2</v>
+      </c>
+      <c r="E23" s="10">
+        <f t="shared" si="2"/>
+        <v>7.6468867269993135E-3</v>
+      </c>
+      <c r="F23" s="11">
+        <f t="shared" si="8"/>
+        <v>0.91669207294837629</v>
+      </c>
+      <c r="G23" s="17">
+        <f t="shared" si="9"/>
+        <v>2120001.2606432312</v>
+      </c>
+      <c r="H23" s="17">
+        <f t="shared" si="10"/>
+        <v>252389660.28064892</v>
+      </c>
+      <c r="I23" s="17">
+        <f t="shared" si="12"/>
+        <v>1169155.7007131237</v>
+      </c>
+      <c r="J23" s="17">
+        <f t="shared" si="3"/>
+        <v>950845.55993010767</v>
+      </c>
+      <c r="K23" s="17">
+        <f t="shared" si="11"/>
+        <v>1929995.14323196</v>
+      </c>
+      <c r="L23" s="17">
+        <f t="shared" si="4"/>
+        <v>4049996.4038751912</v>
+      </c>
+      <c r="M23" s="17">
+        <f t="shared" si="5"/>
+        <v>105649.50665890085</v>
+      </c>
+      <c r="N23" s="17">
+        <f t="shared" si="6"/>
+        <v>3944346.8972162902</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" s="8">
+        <v>23</v>
+      </c>
+      <c r="B24" s="17">
+        <f t="shared" si="7"/>
+        <v>250459665.13741696</v>
+      </c>
+      <c r="C24" s="9">
+        <f t="shared" si="0"/>
+        <v>4.6000000000000006E-2</v>
+      </c>
+      <c r="D24" s="9">
+        <f t="shared" si="1"/>
+        <v>9.2000000000000012E-2</v>
+      </c>
+      <c r="E24" s="10">
+        <f t="shared" si="2"/>
+        <v>8.0103200541153941E-3</v>
+      </c>
+      <c r="F24" s="11">
+        <f t="shared" si="8"/>
+        <v>0.90934907605298931</v>
+      </c>
+      <c r="G24" s="17">
+        <f t="shared" si="9"/>
+        <v>2103789.8511419967</v>
+      </c>
+      <c r="H24" s="17">
+        <f t="shared" si="10"/>
+        <v>249295099.03054029</v>
+      </c>
+      <c r="I24" s="17">
+        <f t="shared" si="12"/>
+        <v>1164566.106876683</v>
+      </c>
+      <c r="J24" s="17">
+        <f t="shared" si="3"/>
+        <v>939223.74426531361</v>
+      </c>
+      <c r="K24" s="17">
+        <f t="shared" si="11"/>
+        <v>1996933.53115702</v>
+      </c>
+      <c r="L24" s="17">
+        <f t="shared" si="4"/>
+        <v>4100723.3822990167</v>
+      </c>
+      <c r="M24" s="17">
+        <f t="shared" si="5"/>
+        <v>104358.19380725706</v>
+      </c>
+      <c r="N24" s="17">
+        <f t="shared" si="6"/>
+        <v>3996365.1884917598</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" s="8">
+        <v>24</v>
+      </c>
+      <c r="B25" s="17">
+        <f t="shared" si="7"/>
+        <v>247298165.49938327</v>
+      </c>
+      <c r="C25" s="9">
+        <f t="shared" si="0"/>
+        <v>4.8000000000000008E-2</v>
+      </c>
+      <c r="D25" s="9">
+        <f t="shared" si="1"/>
+        <v>9.6000000000000016E-2</v>
+      </c>
+      <c r="E25" s="10">
+        <f t="shared" si="2"/>
+        <v>8.3752239642919113E-3</v>
+      </c>
+      <c r="F25" s="11">
+        <f t="shared" si="8"/>
+        <v>0.90173307387932355</v>
+      </c>
+      <c r="G25" s="17">
+        <f t="shared" si="9"/>
+        <v>2086937.8211077496</v>
+      </c>
+      <c r="H25" s="17">
+        <f t="shared" si="10"/>
+        <v>246138595.79889822</v>
+      </c>
+      <c r="I25" s="17">
+        <f t="shared" si="12"/>
+        <v>1159569.7004850623</v>
+      </c>
+      <c r="J25" s="17">
+        <f t="shared" si="3"/>
+        <v>927368.12062268727</v>
+      </c>
+      <c r="K25" s="17">
+        <f t="shared" si="11"/>
+        <v>2061465.8660720927</v>
+      </c>
+      <c r="L25" s="17">
+        <f t="shared" si="4"/>
+        <v>4148403.687179842</v>
+      </c>
+      <c r="M25" s="17">
+        <f t="shared" si="5"/>
+        <v>103040.9022914097</v>
+      </c>
+      <c r="N25" s="17">
+        <f t="shared" si="6"/>
+        <v>4045362.7848884324</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" s="8">
+        <v>25</v>
+      </c>
+      <c r="B26" s="17">
+        <f t="shared" si="7"/>
+        <v>244077129.93282613</v>
+      </c>
+      <c r="C26" s="9">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
+      </c>
+      <c r="D26" s="9">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="E26" s="10">
+        <f t="shared" si="2"/>
+        <v>8.7416109546967213E-3</v>
+      </c>
+      <c r="F26" s="11">
+        <f t="shared" si="8"/>
+        <v>0.89385047416248775</v>
+      </c>
+      <c r="G26" s="17">
+        <f t="shared" si="9"/>
+        <v>2069459.2494564205</v>
+      </c>
+      <c r="H26" s="17">
+        <f t="shared" si="10"/>
+        <v>242922959.92061782</v>
+      </c>
+      <c r="I26" s="17">
+        <f t="shared" si="12"/>
+        <v>1154170.0122083225</v>
+      </c>
+      <c r="J26" s="17">
+        <f t="shared" si="3"/>
+        <v>915289.23724809801</v>
+      </c>
+      <c r="K26" s="17">
+        <f t="shared" si="11"/>
+        <v>2123538.0075894254</v>
+      </c>
+      <c r="L26" s="17">
+        <f t="shared" si="4"/>
+        <v>4192997.257045846</v>
+      </c>
+      <c r="M26" s="17">
+        <f t="shared" si="5"/>
+        <v>101698.80413867754</v>
+      </c>
+      <c r="N26" s="17">
+        <f t="shared" si="6"/>
+        <v>4091298.4529071683</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" s="8">
+        <v>26</v>
+      </c>
+      <c r="B27" s="17">
+        <f t="shared" si="7"/>
+        <v>240799421.91302839</v>
+      </c>
+      <c r="C27" s="9">
+        <f t="shared" si="0"/>
+        <v>5.2000000000000005E-2</v>
+      </c>
+      <c r="D27" s="9">
+        <f t="shared" si="1"/>
+        <v>0.10400000000000001</v>
+      </c>
+      <c r="E27" s="10">
+        <f t="shared" si="2"/>
+        <v>9.109493684829828E-3</v>
+      </c>
+      <c r="F27" s="11">
+        <f t="shared" si="8"/>
+        <v>0.88570794891292237</v>
+      </c>
+      <c r="G27" s="17">
+        <f t="shared" si="9"/>
+        <v>2051368.8418110739</v>
+      </c>
+      <c r="H27" s="17">
+        <f t="shared" si="10"/>
+        <v>239651050.90339118</v>
+      </c>
+      <c r="I27" s="17">
+        <f t="shared" si="12"/>
+        <v>1148371.0096372175</v>
+      </c>
+      <c r="J27" s="17">
+        <f t="shared" si="3"/>
+        <v>902997.83217385644</v>
+      </c>
+      <c r="K27" s="17">
+        <f t="shared" si="11"/>
+        <v>2183099.7347672735</v>
+      </c>
+      <c r="L27" s="17">
+        <f t="shared" si="4"/>
+        <v>4234468.576578347</v>
+      </c>
+      <c r="M27" s="17">
+        <f t="shared" si="5"/>
+        <v>100333.09246376182</v>
+      </c>
+      <c r="N27" s="17">
+        <f t="shared" si="6"/>
+        <v>4134135.484114585</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28" s="8">
+        <v>27</v>
+      </c>
+      <c r="B28" s="17">
+        <f t="shared" si="7"/>
+        <v>237467951.16862389</v>
+      </c>
+      <c r="C28" s="9">
+        <f t="shared" si="0"/>
+        <v>5.4000000000000006E-2</v>
+      </c>
+      <c r="D28" s="9">
+        <f t="shared" si="1"/>
+        <v>0.10800000000000001</v>
+      </c>
+      <c r="E28" s="10">
+        <f t="shared" si="2"/>
+        <v>9.4788849793674412E-3</v>
+      </c>
+      <c r="F28" s="11">
+        <f t="shared" si="8"/>
+        <v>0.87731242513986529</v>
+      </c>
+      <c r="G28" s="17">
+        <f t="shared" si="9"/>
+        <v>2032681.9103013391</v>
+      </c>
+      <c r="H28" s="17">
+        <f t="shared" si="10"/>
+        <v>236325774.07520491</v>
+      </c>
+      <c r="I28" s="17">
+        <f t="shared" si="12"/>
+        <v>1142177.0934189996</v>
+      </c>
+      <c r="J28" s="17">
+        <f t="shared" si="3"/>
+        <v>890504.81688233954</v>
+      </c>
+      <c r="K28" s="17">
+        <f t="shared" si="11"/>
+        <v>2240104.8301188434</v>
+      </c>
+      <c r="L28" s="17">
+        <f t="shared" si="4"/>
+        <v>4272786.7404201822</v>
+      </c>
+      <c r="M28" s="17">
+        <f t="shared" si="5"/>
+        <v>98944.979653593284</v>
+      </c>
+      <c r="N28" s="17">
+        <f t="shared" si="6"/>
+        <v>4173841.7607665891</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29" s="8">
+        <v>28</v>
+      </c>
+      <c r="B29" s="17">
+        <f t="shared" si="7"/>
+        <v>234085669.24508607</v>
+      </c>
+      <c r="C29" s="9">
+        <f t="shared" si="0"/>
+        <v>5.6000000000000008E-2</v>
+      </c>
+      <c r="D29" s="9">
+        <f t="shared" si="1"/>
+        <v>0.11200000000000002</v>
+      </c>
+      <c r="E29" s="10">
+        <f t="shared" si="2"/>
+        <v>9.84979783106954E-3</v>
+      </c>
+      <c r="F29" s="11">
+        <f t="shared" si="8"/>
+        <v>0.86867107511755226</v>
+      </c>
+      <c r="G29" s="17">
+        <f t="shared" si="9"/>
+        <v>2013414.3522739518</v>
+      </c>
+      <c r="H29" s="17">
+        <f t="shared" si="10"/>
+        <v>232950076.1524812</v>
+      </c>
+      <c r="I29" s="17">
+        <f t="shared" si="12"/>
+        <v>1135593.0926048791</v>
+      </c>
+      <c r="J29" s="17">
+        <f t="shared" si="3"/>
+        <v>877821.25966907269</v>
+      </c>
+      <c r="K29" s="17">
+        <f t="shared" si="11"/>
+        <v>2294511.1548341936</v>
+      </c>
+      <c r="L29" s="17">
+        <f t="shared" si="4"/>
+        <v>4307925.5071081454</v>
+      </c>
+      <c r="M29" s="17">
+        <f t="shared" si="5"/>
+        <v>97535.695518785855</v>
+      </c>
+      <c r="N29" s="17">
+        <f t="shared" si="6"/>
+        <v>4210389.8115893593</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30" s="8">
+        <v>29</v>
+      </c>
+      <c r="B30" s="17">
+        <f t="shared" si="7"/>
+        <v>230655564.99764702</v>
+      </c>
+      <c r="C30" s="9">
+        <f t="shared" si="0"/>
+        <v>5.800000000000001E-2</v>
+      </c>
+      <c r="D30" s="9">
+        <f t="shared" si="1"/>
+        <v>0.11600000000000002</v>
+      </c>
+      <c r="E30" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0222245403750829E-2</v>
+      </c>
+      <c r="F30" s="11">
+        <f t="shared" si="8"/>
+        <v>0.85979130621256061</v>
+      </c>
+      <c r="G30" s="17">
+        <f t="shared" si="9"/>
+        <v>1993582.6279538795</v>
+      </c>
+      <c r="H30" s="17">
+        <f t="shared" si="10"/>
+        <v>229526940.73843431</v>
+      </c>
+      <c r="I30" s="17">
+        <f t="shared" si="12"/>
+        <v>1128624.2592127032</v>
+      </c>
+      <c r="J30" s="17">
+        <f t="shared" si="3"/>
+        <v>864958.36874117632</v>
+      </c>
+      <c r="K30" s="17">
+        <f t="shared" si="11"/>
+        <v>2346280.7150004492</v>
+      </c>
+      <c r="L30" s="17">
+        <f t="shared" si="4"/>
+        <v>4339863.3429543283</v>
+      </c>
+      <c r="M30" s="17">
+        <f t="shared" si="5"/>
+        <v>96106.485415686257</v>
+      </c>
+      <c r="N30" s="17">
+        <f t="shared" si="6"/>
+        <v>4243756.8575386424</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31" s="8">
+        <v>30</v>
+      </c>
+      <c r="B31" s="17">
+        <f t="shared" si="7"/>
+        <v>227180660.02343386</v>
+      </c>
+      <c r="C31" s="9">
+        <f t="shared" si="0"/>
+        <v>0.06</v>
+      </c>
+      <c r="D31" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E31" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F31" s="11">
+        <f t="shared" si="8"/>
+        <v>0.85068075029186052</v>
+      </c>
+      <c r="G31" s="17">
+        <f t="shared" si="9"/>
+        <v>1973203.7370982806</v>
+      </c>
+      <c r="H31" s="17">
+        <f t="shared" si="10"/>
+        <v>226059383.76142347</v>
+      </c>
+      <c r="I31" s="17">
+        <f t="shared" si="12"/>
+        <v>1121276.2620104034</v>
+      </c>
+      <c r="J31" s="17">
+        <f t="shared" si="3"/>
+        <v>851927.47508787701</v>
+      </c>
+      <c r="K31" s="17">
+        <f t="shared" si="11"/>
+        <v>2395379.7186317155</v>
+      </c>
+      <c r="L31" s="17">
+        <f t="shared" si="4"/>
+        <v>4368583.4557299959</v>
+      </c>
+      <c r="M31" s="17">
+        <f t="shared" si="5"/>
+        <v>94658.608343097454</v>
+      </c>
+      <c r="N31" s="17">
+        <f t="shared" si="6"/>
+        <v>4273924.8473868985</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A32" s="8">
+        <v>31</v>
+      </c>
+      <c r="B32" s="17">
+        <f t="shared" si="7"/>
+        <v>223664004.04279175</v>
+      </c>
+      <c r="C32" s="9">
+        <f>C31</f>
+        <v>0.06</v>
+      </c>
+      <c r="D32" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E32" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F32" s="11">
+        <f t="shared" si="8"/>
+        <v>0.84166673201766196</v>
+      </c>
+      <c r="G32" s="17">
+        <f t="shared" si="9"/>
+        <v>1952295.1946881949</v>
+      </c>
+      <c r="H32" s="17">
+        <f t="shared" si="10"/>
+        <v>222550448.86326402</v>
+      </c>
+      <c r="I32" s="17">
+        <f t="shared" si="12"/>
+        <v>1113555.179527726</v>
+      </c>
+      <c r="J32" s="17">
+        <f t="shared" si="3"/>
+        <v>838740.01516046899</v>
+      </c>
+      <c r="K32" s="17">
+        <f t="shared" si="11"/>
+        <v>2358198.1986735757</v>
+      </c>
+      <c r="L32" s="17">
+        <f t="shared" si="4"/>
+        <v>4310493.3933617705</v>
+      </c>
+      <c r="M32" s="17">
+        <f t="shared" si="5"/>
+        <v>93193.335017829901</v>
+      </c>
+      <c r="N32" s="17">
+        <f t="shared" si="6"/>
+        <v>4217300.0583439404</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A33" s="8">
+        <v>32</v>
+      </c>
+      <c r="B33" s="17">
+        <f t="shared" si="7"/>
+        <v>220192250.66459045</v>
+      </c>
+      <c r="C33" s="9">
+        <f t="shared" ref="C33:C62" si="13">C32</f>
+        <v>0.06</v>
+      </c>
+      <c r="D33" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E33" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F33" s="11">
+        <f t="shared" si="8"/>
+        <v>0.83274822845379359</v>
+      </c>
+      <c r="G33" s="17">
+        <f t="shared" si="9"/>
+        <v>1931608.2042331838</v>
+      </c>
+      <c r="H33" s="17">
+        <f t="shared" si="10"/>
+        <v>219086363.40034947</v>
+      </c>
+      <c r="I33" s="17">
+        <f t="shared" si="12"/>
+        <v>1105887.2642409694</v>
+      </c>
+      <c r="J33" s="17">
+        <f t="shared" si="3"/>
+        <v>825720.9399922142</v>
+      </c>
+      <c r="K33" s="17">
+        <f t="shared" si="11"/>
+        <v>2321491.9141415884</v>
+      </c>
+      <c r="L33" s="17">
+        <f t="shared" si="4"/>
+        <v>4253100.1183747724</v>
+      </c>
+      <c r="M33" s="17">
+        <f t="shared" si="5"/>
+        <v>91746.771110246016</v>
+      </c>
+      <c r="N33" s="17">
+        <f t="shared" si="6"/>
+        <v>4161353.3472645264</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34" s="8">
+        <v>33</v>
+      </c>
+      <c r="B34" s="17">
+        <f t="shared" si="7"/>
+        <v>216764871.48620787</v>
+      </c>
+      <c r="C34" s="9">
+        <f t="shared" si="13"/>
+        <v>0.06</v>
+      </c>
+      <c r="D34" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E34" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F34" s="11">
+        <f t="shared" si="8"/>
+        <v>0.82392422750336236</v>
+      </c>
+      <c r="G34" s="17">
+        <f t="shared" si="9"/>
+        <v>1911140.4181153292</v>
+      </c>
+      <c r="H34" s="17">
+        <f t="shared" si="10"/>
+        <v>215666599.33616582</v>
+      </c>
+      <c r="I34" s="17">
+        <f t="shared" si="12"/>
+        <v>1098272.1500420496</v>
+      </c>
+      <c r="J34" s="17">
+        <f t="shared" si="3"/>
+        <v>812868.26807327953</v>
+      </c>
+      <c r="K34" s="17">
+        <f t="shared" si="11"/>
+        <v>2285255.2698335764</v>
+      </c>
+      <c r="L34" s="17">
+        <f t="shared" si="4"/>
+        <v>4196395.6879489049</v>
+      </c>
+      <c r="M34" s="17">
+        <f t="shared" si="5"/>
+        <v>90318.696452586621</v>
+      </c>
+      <c r="N34" s="17">
+        <f t="shared" si="6"/>
+        <v>4106076.9914963185</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35" s="8">
+        <v>34</v>
+      </c>
+      <c r="B35" s="17">
+        <f t="shared" si="7"/>
+        <v>213381344.06633225</v>
+      </c>
+      <c r="C35" s="9">
+        <f t="shared" si="13"/>
+        <v>0.06</v>
+      </c>
+      <c r="D35" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E35" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F35" s="11">
+        <f t="shared" si="8"/>
+        <v>0.81519372779389776</v>
+      </c>
+      <c r="G35" s="17">
+        <f t="shared" si="9"/>
+        <v>1890889.513592639</v>
+      </c>
+      <c r="H35" s="17">
+        <f t="shared" si="10"/>
+        <v>212290634.59298837</v>
+      </c>
+      <c r="I35" s="17">
+        <f t="shared" si="12"/>
+        <v>1090709.473343893</v>
+      </c>
+      <c r="J35" s="17">
+        <f t="shared" si="3"/>
+        <v>800180.04024874594</v>
+      </c>
+      <c r="K35" s="17">
+        <f t="shared" si="11"/>
+        <v>2249482.7336881296</v>
+      </c>
+      <c r="L35" s="17">
+        <f t="shared" si="4"/>
+        <v>4140372.2472807686</v>
+      </c>
+      <c r="M35" s="17">
+        <f t="shared" si="5"/>
+        <v>88908.893360971764</v>
+      </c>
+      <c r="N35" s="17">
+        <f t="shared" si="6"/>
+        <v>4051463.3539197966</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36" s="8">
+        <v>35</v>
+      </c>
+      <c r="B36" s="17">
+        <f t="shared" si="7"/>
+        <v>210041151.85930026</v>
+      </c>
+      <c r="C36" s="9">
+        <f t="shared" si="13"/>
+        <v>0.06</v>
+      </c>
+      <c r="D36" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E36" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F36" s="11">
+        <f t="shared" si="8"/>
+        <v>0.80655573856371343</v>
+      </c>
+      <c r="G36" s="17">
+        <f t="shared" si="9"/>
+        <v>1870853.1925354544</v>
+      </c>
+      <c r="H36" s="17">
+        <f t="shared" si="10"/>
+        <v>208957952.98623717</v>
+      </c>
+      <c r="I36" s="17">
+        <f t="shared" si="12"/>
+        <v>1083198.8730630786</v>
+      </c>
+      <c r="J36" s="17">
+        <f t="shared" si="3"/>
+        <v>787654.31947237591</v>
+      </c>
+      <c r="K36" s="17">
+        <f t="shared" si="11"/>
+        <v>2214168.8360890197</v>
+      </c>
+      <c r="L36" s="17">
+        <f t="shared" si="4"/>
+        <v>4085022.0286244741</v>
+      </c>
+      <c r="M36" s="17">
+        <f t="shared" si="5"/>
+        <v>87517.146608041774</v>
+      </c>
+      <c r="N36" s="17">
+        <f t="shared" si="6"/>
+        <v>3997504.8820164325</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A37" s="8">
+        <v>36</v>
+      </c>
+      <c r="B37" s="17">
+        <f t="shared" si="7"/>
+        <v>206743784.15014815</v>
+      </c>
+      <c r="C37" s="9">
+        <f t="shared" si="13"/>
+        <v>0.06</v>
+      </c>
+      <c r="D37" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E37" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F37" s="11">
+        <f t="shared" si="8"/>
+        <v>0.79800927954947265</v>
+      </c>
+      <c r="G37" s="17">
+        <f t="shared" si="9"/>
+        <v>1851029.1811656528</v>
+      </c>
+      <c r="H37" s="17">
+        <f t="shared" si="10"/>
+        <v>205668044.15954557</v>
+      </c>
+      <c r="I37" s="17">
+        <f t="shared" si="12"/>
+        <v>1075739.9906025971</v>
+      </c>
+      <c r="J37" s="17">
+        <f t="shared" si="3"/>
+        <v>775289.19056305557</v>
+      </c>
+      <c r="K37" s="17">
+        <f t="shared" si="11"/>
+        <v>2179308.1691771722</v>
+      </c>
+      <c r="L37" s="17">
+        <f t="shared" si="4"/>
+        <v>4030337.3503428251</v>
+      </c>
+      <c r="M37" s="17">
+        <f t="shared" si="5"/>
+        <v>86143.243395895071</v>
+      </c>
+      <c r="N37" s="17">
+        <f t="shared" si="6"/>
+        <v>3944194.1069469298</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A38" s="8">
+        <v>37</v>
+      </c>
+      <c r="B38" s="17">
+        <f t="shared" si="7"/>
+        <v>203488735.9903684</v>
+      </c>
+      <c r="C38" s="9">
+        <f t="shared" si="13"/>
+        <v>0.06</v>
+      </c>
+      <c r="D38" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E38" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F38" s="11">
+        <f t="shared" si="8"/>
+        <v>0.7895533808749452</v>
+      </c>
+      <c r="G38" s="17">
+        <f t="shared" si="9"/>
+        <v>1831415.2297986127</v>
+      </c>
+      <c r="H38" s="17">
+        <f t="shared" si="10"/>
+        <v>202420403.52053365</v>
+      </c>
+      <c r="I38" s="17">
+        <f t="shared" si="12"/>
+        <v>1068332.4698347312</v>
+      </c>
+      <c r="J38" s="17">
+        <f t="shared" si="3"/>
+        <v>763082.75996388146</v>
+      </c>
+      <c r="K38" s="17">
+        <f t="shared" si="11"/>
+        <v>2144895.3861701046</v>
+      </c>
+      <c r="L38" s="17">
+        <f t="shared" si="4"/>
+        <v>3976310.6159687173</v>
+      </c>
+      <c r="M38" s="17">
+        <f t="shared" si="5"/>
+        <v>84786.973329320157</v>
+      </c>
+      <c r="N38" s="17">
+        <f t="shared" si="6"/>
+        <v>3891523.6426393972</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A39" s="8">
+        <v>38</v>
+      </c>
+      <c r="B39" s="17">
+        <f t="shared" si="7"/>
+        <v>200275508.13436353</v>
+      </c>
+      <c r="C39" s="9">
+        <f t="shared" si="13"/>
+        <v>0.06</v>
+      </c>
+      <c r="D39" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E39" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F39" s="11">
+        <f t="shared" si="8"/>
+        <v>0.7811870829409433</v>
+      </c>
+      <c r="G39" s="17">
+        <f t="shared" si="9"/>
+        <v>1812009.1125879122</v>
+      </c>
+      <c r="H39" s="17">
+        <f t="shared" si="10"/>
+        <v>199214532.17727947</v>
+      </c>
+      <c r="I39" s="17">
+        <f t="shared" si="12"/>
+        <v>1060975.957084049</v>
+      </c>
+      <c r="J39" s="17">
+        <f t="shared" si="3"/>
+        <v>751033.15550386324</v>
+      </c>
+      <c r="K39" s="17">
+        <f t="shared" si="11"/>
+        <v>2110925.2006887612</v>
+      </c>
+      <c r="L39" s="17">
+        <f t="shared" si="4"/>
+        <v>3922934.3132766737</v>
+      </c>
+      <c r="M39" s="17">
+        <f t="shared" si="5"/>
+        <v>83448.128389318139</v>
+      </c>
+      <c r="N39" s="17">
+        <f t="shared" si="6"/>
+        <v>3839486.1848873557</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A40" s="8">
+        <v>39</v>
+      </c>
+      <c r="B40" s="17">
+        <f t="shared" si="7"/>
+        <v>197103606.97659072</v>
+      </c>
+      <c r="C40" s="9">
+        <f t="shared" si="13"/>
+        <v>0.06</v>
+      </c>
+      <c r="D40" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E40" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F40" s="11">
+        <f t="shared" si="8"/>
+        <v>0.77290943631642339</v>
+      </c>
+      <c r="G40" s="17">
+        <f t="shared" si="9"/>
+        <v>1792808.6272727365</v>
+      </c>
+      <c r="H40" s="17">
+        <f t="shared" si="10"/>
+        <v>196049936.8754802</v>
+      </c>
+      <c r="I40" s="17">
+        <f t="shared" si="12"/>
+        <v>1053670.1011105212</v>
+      </c>
+      <c r="J40" s="17">
+        <f t="shared" si="3"/>
+        <v>739138.52616221516</v>
+      </c>
+      <c r="K40" s="17">
+        <f t="shared" si="11"/>
+        <v>2077392.3860916584</v>
+      </c>
+      <c r="L40" s="17">
+        <f t="shared" si="4"/>
+        <v>3870201.0133643947</v>
+      </c>
+      <c r="M40" s="17">
+        <f t="shared" si="5"/>
+        <v>82126.502906912807</v>
+      </c>
+      <c r="N40" s="17">
+        <f t="shared" si="6"/>
+        <v>3788074.5104574817</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A41" s="8">
+        <v>40</v>
+      </c>
+      <c r="B41" s="17">
+        <f t="shared" si="7"/>
+        <v>193972544.48938856</v>
+      </c>
+      <c r="C41" s="9">
+        <f t="shared" si="13"/>
+        <v>0.06</v>
+      </c>
+      <c r="D41" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E41" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F41" s="11">
+        <f t="shared" si="8"/>
+        <v>0.76471950163074209</v>
+      </c>
+      <c r="G41" s="17">
+        <f t="shared" si="9"/>
+        <v>1773811.5949279554</v>
+      </c>
+      <c r="H41" s="17">
+        <f t="shared" si="10"/>
+        <v>192926129.93629581</v>
+      </c>
+      <c r="I41" s="17">
+        <f t="shared" si="12"/>
+        <v>1046414.5530927484</v>
+      </c>
+      <c r="J41" s="17">
+        <f t="shared" si="3"/>
+        <v>727397.04183520703</v>
+      </c>
+      <c r="K41" s="17">
+        <f t="shared" si="11"/>
+        <v>2044291.7748162583</v>
+      </c>
+      <c r="L41" s="17">
+        <f t="shared" si="4"/>
+        <v>3818103.3697442138</v>
+      </c>
+      <c r="M41" s="17">
+        <f t="shared" si="5"/>
+        <v>80821.893537245225</v>
+      </c>
+      <c r="N41" s="17">
+        <f t="shared" si="6"/>
+        <v>3737281.4762069685</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A42" s="8">
+        <v>41</v>
+      </c>
+      <c r="B42" s="17">
+        <f t="shared" si="7"/>
+        <v>190881838.16147956</v>
+      </c>
+      <c r="C42" s="9">
+        <f t="shared" si="13"/>
+        <v>0.06</v>
+      </c>
+      <c r="D42" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E42" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F42" s="11">
+        <f t="shared" si="8"/>
+        <v>0.75661634946705369</v>
+      </c>
+      <c r="G42" s="17">
+        <f t="shared" si="9"/>
+        <v>1755015.8597168552</v>
+      </c>
+      <c r="H42" s="17">
+        <f t="shared" si="10"/>
+        <v>189842629.19486827</v>
+      </c>
+      <c r="I42" s="17">
+        <f t="shared" si="12"/>
+        <v>1039208.9666113069</v>
+      </c>
+      <c r="J42" s="17">
+        <f t="shared" si="3"/>
+        <v>715806.89310554834</v>
+      </c>
+      <c r="K42" s="17">
+        <f t="shared" si="11"/>
+        <v>2011618.2577275075</v>
+      </c>
+      <c r="L42" s="17">
+        <f t="shared" si="4"/>
+        <v>3766634.1174443625</v>
+      </c>
+      <c r="M42" s="17">
+        <f t="shared" si="5"/>
+        <v>79534.099233949819</v>
+      </c>
+      <c r="N42" s="17">
+        <f t="shared" si="6"/>
+        <v>3687100.0182104125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A43" s="8">
+        <v>42</v>
+      </c>
+      <c r="B43" s="17">
+        <f t="shared" si="7"/>
+        <v>187831010.93714076</v>
+      </c>
+      <c r="C43" s="9">
+        <f t="shared" si="13"/>
+        <v>0.06</v>
+      </c>
+      <c r="D43" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E43" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F43" s="11">
+        <f t="shared" si="8"/>
+        <v>0.74859906025683765</v>
+      </c>
+      <c r="G43" s="17">
+        <f t="shared" si="9"/>
+        <v>1736419.2886464878</v>
+      </c>
+      <c r="H43" s="17">
+        <f t="shared" si="10"/>
+        <v>186798957.93950856</v>
+      </c>
+      <c r="I43" s="17">
+        <f t="shared" si="12"/>
+        <v>1032052.9976322099</v>
+      </c>
+      <c r="J43" s="17">
+        <f t="shared" si="3"/>
+        <v>704366.29101427784</v>
+      </c>
+      <c r="K43" s="17">
+        <f t="shared" si="11"/>
+        <v>1979366.7834734439</v>
+      </c>
+      <c r="L43" s="17">
+        <f t="shared" si="4"/>
+        <v>3715786.0721199317</v>
+      </c>
+      <c r="M43" s="17">
+        <f t="shared" si="5"/>
+        <v>78262.921223808647</v>
+      </c>
+      <c r="N43" s="17">
+        <f t="shared" si="6"/>
+        <v>3637523.1508961231</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A44" s="8">
+        <v>43</v>
+      </c>
+      <c r="B44" s="17">
+        <f t="shared" si="7"/>
+        <v>184819591.15603513</v>
+      </c>
+      <c r="C44" s="9">
+        <f t="shared" si="13"/>
+        <v>0.06</v>
+      </c>
+      <c r="D44" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E44" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F44" s="11">
+        <f t="shared" si="8"/>
+        <v>0.74066672417554291</v>
+      </c>
+      <c r="G44" s="17">
+        <f t="shared" si="9"/>
+        <v>1718019.7713256124</v>
+      </c>
+      <c r="H44" s="17">
+        <f t="shared" si="10"/>
+        <v>183794644.85154465</v>
+      </c>
+      <c r="I44" s="17">
+        <f t="shared" si="12"/>
+        <v>1024946.3044904808</v>
+      </c>
+      <c r="J44" s="17">
+        <f t="shared" si="3"/>
+        <v>693073.46683513164</v>
+      </c>
+      <c r="K44" s="17">
+        <f t="shared" si="11"/>
+        <v>1947532.3578478149</v>
+      </c>
+      <c r="L44" s="17">
+        <f t="shared" si="4"/>
+        <v>3665552.1291734274</v>
+      </c>
+      <c r="M44" s="17">
+        <f t="shared" si="5"/>
+        <v>77008.162981681293</v>
+      </c>
+      <c r="N44" s="17">
+        <f t="shared" si="6"/>
+        <v>3588543.9661917463</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A45" s="8">
+        <v>44</v>
+      </c>
+      <c r="B45" s="17">
+        <f t="shared" si="7"/>
+        <v>181847112.49369684</v>
+      </c>
+      <c r="C45" s="9">
+        <f t="shared" si="13"/>
+        <v>0.06</v>
+      </c>
+      <c r="D45" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E45" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F45" s="11">
+        <f t="shared" si="8"/>
+        <v>0.7328184410393388</v>
+      </c>
+      <c r="G45" s="17">
+        <f t="shared" si="9"/>
+        <v>1699815.2197252025</v>
+      </c>
+      <c r="H45" s="17">
+        <f t="shared" si="10"/>
+        <v>180829223.94582301</v>
+      </c>
+      <c r="I45" s="17">
+        <f t="shared" si="12"/>
+        <v>1017888.5478738394</v>
+      </c>
+      <c r="J45" s="17">
+        <f t="shared" si="3"/>
+        <v>681926.67185136315</v>
+      </c>
+      <c r="K45" s="17">
+        <f t="shared" si="11"/>
+        <v>1916110.0431596145</v>
+      </c>
+      <c r="L45" s="17">
+        <f t="shared" si="4"/>
+        <v>3615925.2628848171</v>
+      </c>
+      <c r="M45" s="17">
+        <f t="shared" si="5"/>
+        <v>75769.630205707013</v>
+      </c>
+      <c r="N45" s="17">
+        <f t="shared" si="6"/>
+        <v>3540155.6326791099</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A46" s="8">
+        <v>45</v>
+      </c>
+      <c r="B46" s="17">
+        <f t="shared" si="7"/>
+        <v>178913113.90266341</v>
+      </c>
+      <c r="C46" s="9">
+        <f t="shared" si="13"/>
+        <v>0.06</v>
+      </c>
+      <c r="D46" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E46" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F46" s="11">
+        <f t="shared" si="8"/>
+        <v>0.72505332020295932</v>
+      </c>
+      <c r="G46" s="17">
+        <f t="shared" si="9"/>
+        <v>1681803.5679414908</v>
+      </c>
+      <c r="H46" s="17">
+        <f t="shared" si="10"/>
+        <v>177902234.51185691</v>
+      </c>
+      <c r="I46" s="17">
+        <f t="shared" si="12"/>
+        <v>1010879.390806503</v>
+      </c>
+      <c r="J46" s="17">
+        <f t="shared" si="3"/>
+        <v>670924.17713498778</v>
+      </c>
+      <c r="K46" s="17">
+        <f t="shared" si="11"/>
+        <v>1885094.9576094779</v>
+      </c>
+      <c r="L46" s="17">
+        <f t="shared" si="4"/>
+        <v>3566898.5255509689</v>
+      </c>
+      <c r="M46" s="17">
+        <f t="shared" si="5"/>
+        <v>74547.130792776428</v>
+      </c>
+      <c r="N46" s="17">
+        <f t="shared" si="6"/>
+        <v>3492351.3947581924</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A47" s="8">
+        <v>46</v>
+      </c>
+      <c r="B47" s="17">
+        <f t="shared" si="7"/>
+        <v>176017139.55424744</v>
+      </c>
+      <c r="C47" s="9">
+        <f t="shared" si="13"/>
+        <v>0.06</v>
+      </c>
+      <c r="D47" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E47" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F47" s="11">
+        <f t="shared" si="8"/>
+        <v>0.7173704804586305</v>
+      </c>
+      <c r="G47" s="17">
+        <f t="shared" si="9"/>
+        <v>1663982.7719615235</v>
+      </c>
+      <c r="H47" s="17">
+        <f t="shared" si="10"/>
+        <v>175013221.05561435</v>
+      </c>
+      <c r="I47" s="17">
+        <f t="shared" si="12"/>
+        <v>1003918.4986330955</v>
+      </c>
+      <c r="J47" s="17">
+        <f t="shared" si="3"/>
+        <v>660064.27332842792</v>
+      </c>
+      <c r="K47" s="17">
+        <f t="shared" si="11"/>
+        <v>1854482.2746728519</v>
+      </c>
+      <c r="L47" s="17">
+        <f t="shared" si="4"/>
+        <v>3518465.0466343751</v>
+      </c>
+      <c r="M47" s="17">
+        <f t="shared" si="5"/>
+        <v>73340.474814269764</v>
+      </c>
+      <c r="N47" s="17">
+        <f t="shared" si="6"/>
+        <v>3445124.5718201054</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A48" s="8">
+        <v>47</v>
+      </c>
+      <c r="B48" s="17">
+        <f t="shared" si="7"/>
+        <v>173158738.78094149</v>
+      </c>
+      <c r="C48" s="9">
+        <f t="shared" si="13"/>
+        <v>0.06</v>
+      </c>
+      <c r="D48" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E48" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F48" s="11">
+        <f t="shared" si="8"/>
+        <v>0.70976904993606826</v>
+      </c>
+      <c r="G48" s="17">
+        <f t="shared" si="9"/>
+        <v>1646350.8094312011</v>
+      </c>
+      <c r="H48" s="17">
+        <f t="shared" si="10"/>
+        <v>172161733.24193883</v>
+      </c>
+      <c r="I48" s="17">
+        <f t="shared" si="12"/>
+        <v>997005.53900267056</v>
+      </c>
+      <c r="J48" s="17">
+        <f t="shared" si="3"/>
+        <v>649345.27042853052</v>
+      </c>
+      <c r="K48" s="17">
+        <f t="shared" si="11"/>
+        <v>1824267.2224898713</v>
+      </c>
+      <c r="L48" s="17">
+        <f t="shared" si="4"/>
+        <v>3470618.0319210724</v>
+      </c>
+      <c r="M48" s="17">
+        <f t="shared" si="5"/>
+        <v>72149.474492058944</v>
+      </c>
+      <c r="N48" s="17">
+        <f t="shared" si="6"/>
+        <v>3398468.5574290133</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A49" s="8">
+        <v>48</v>
+      </c>
+      <c r="B49" s="17">
+        <f t="shared" si="7"/>
+        <v>170337466.01944897</v>
+      </c>
+      <c r="C49" s="9">
+        <f t="shared" si="13"/>
+        <v>0.06</v>
+      </c>
+      <c r="D49" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E49" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F49" s="11">
+        <f t="shared" si="8"/>
+        <v>0.70224816600353634</v>
+      </c>
+      <c r="G49" s="17">
+        <f t="shared" si="9"/>
+        <v>1628905.6794257755</v>
+      </c>
+      <c r="H49" s="17">
+        <f t="shared" si="10"/>
+        <v>169347325.83759612</v>
+      </c>
+      <c r="I49" s="17">
+        <f t="shared" si="12"/>
+        <v>990140.18185284198</v>
+      </c>
+      <c r="J49" s="17">
+        <f t="shared" si="3"/>
+        <v>638765.49757293356</v>
+      </c>
+      <c r="K49" s="17">
+        <f t="shared" si="11"/>
+        <v>1794445.0832618696</v>
+      </c>
+      <c r="L49" s="17">
+        <f t="shared" si="4"/>
+        <v>3423350.7626876449</v>
+      </c>
+      <c r="M49" s="17">
+        <f t="shared" si="5"/>
+        <v>70973.944174770397</v>
+      </c>
+      <c r="N49" s="17">
+        <f t="shared" si="6"/>
+        <v>3352376.8185128747</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A50" s="8">
+        <v>49</v>
+      </c>
+      <c r="B50" s="17">
+        <f t="shared" si="7"/>
+        <v>167552880.75433424</v>
+      </c>
+      <c r="C50" s="9">
+        <f t="shared" si="13"/>
+        <v>0.06</v>
+      </c>
+      <c r="D50" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E50" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F50" s="11">
+        <f t="shared" si="8"/>
+        <v>0.69480697516995216</v>
+      </c>
+      <c r="G50" s="17">
+        <f t="shared" si="9"/>
+        <v>1611645.40222278</v>
+      </c>
+      <c r="H50" s="17">
+        <f t="shared" si="10"/>
+        <v>166569558.65494022</v>
+      </c>
+      <c r="I50" s="17">
+        <f t="shared" si="12"/>
+        <v>983322.09939402668</v>
+      </c>
+      <c r="J50" s="17">
+        <f t="shared" si="3"/>
+        <v>628323.30282875337</v>
+      </c>
+      <c r="K50" s="17">
+        <f t="shared" si="11"/>
+        <v>1765011.1926544486</v>
+      </c>
+      <c r="L50" s="17">
+        <f t="shared" si="4"/>
+        <v>3376656.5948772286</v>
+      </c>
+      <c r="M50" s="17">
+        <f t="shared" si="5"/>
+        <v>69813.700314305926</v>
+      </c>
+      <c r="N50" s="17">
+        <f t="shared" si="6"/>
+        <v>3306842.8945629229</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A51" s="8">
+        <v>50</v>
+      </c>
+      <c r="B51" s="17">
+        <f t="shared" si="7"/>
+        <v>164804547.46228576</v>
+      </c>
+      <c r="C51" s="9">
+        <f t="shared" si="13"/>
+        <v>0.06</v>
+      </c>
+      <c r="D51" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E51" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F51" s="11">
+        <f t="shared" si="8"/>
+        <v>0.68744463298803049</v>
+      </c>
+      <c r="G51" s="17">
+        <f t="shared" si="9"/>
+        <v>1594568.0190773637</v>
+      </c>
+      <c r="H51" s="17">
+        <f t="shared" si="10"/>
+        <v>163827996.49619198</v>
+      </c>
+      <c r="I51" s="17">
+        <f t="shared" si="12"/>
+        <v>976550.96609379211</v>
+      </c>
+      <c r="J51" s="17">
+        <f t="shared" si="3"/>
+        <v>618017.05298357154</v>
+      </c>
+      <c r="K51" s="17">
+        <f t="shared" si="11"/>
+        <v>1735960.9392070428</v>
+      </c>
+      <c r="L51" s="17">
+        <f t="shared" si="4"/>
+        <v>3330528.9582844065</v>
+      </c>
+      <c r="M51" s="17">
+        <f t="shared" si="5"/>
+        <v>68668.561442619073</v>
+      </c>
+      <c r="N51" s="17">
+        <f t="shared" si="6"/>
+        <v>3261860.3968417873</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A52" s="8">
+        <v>51</v>
+      </c>
+      <c r="B52" s="17">
+        <f t="shared" si="7"/>
+        <v>162092035.55698493</v>
+      </c>
+      <c r="C52" s="9">
+        <f t="shared" si="13"/>
+        <v>0.06</v>
+      </c>
+      <c r="D52" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E52" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F52" s="11">
+        <f t="shared" si="8"/>
+        <v>0.68016030395845295</v>
+      </c>
+      <c r="G52" s="17">
+        <f t="shared" si="9"/>
+        <v>1577671.592000009</v>
+      </c>
+      <c r="H52" s="17">
+        <f t="shared" si="10"/>
+        <v>161122209.09832361</v>
+      </c>
+      <c r="I52" s="17">
+        <f t="shared" si="12"/>
+        <v>969826.45866131561</v>
+      </c>
+      <c r="J52" s="17">
+        <f t="shared" si="3"/>
+        <v>607845.13333869341</v>
+      </c>
+      <c r="K52" s="17">
+        <f t="shared" si="11"/>
+        <v>1707289.7637489012</v>
+      </c>
+      <c r="L52" s="17">
+        <f t="shared" si="4"/>
+        <v>3284961.3557489105</v>
+      </c>
+      <c r="M52" s="17">
+        <f t="shared" si="5"/>
+        <v>67538.348148743724</v>
+      </c>
+      <c r="N52" s="17">
+        <f t="shared" si="6"/>
+        <v>3217423.0076001668</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A53" s="8">
+        <v>52</v>
+      </c>
+      <c r="B53" s="17">
+        <f t="shared" si="7"/>
+        <v>159414919.3345747</v>
+      </c>
+      <c r="C53" s="9">
+        <f t="shared" si="13"/>
+        <v>0.06</v>
+      </c>
+      <c r="D53" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E53" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F53" s="11">
+        <f t="shared" si="8"/>
+        <v>0.67295316143505335</v>
+      </c>
+      <c r="G53" s="17">
+        <f t="shared" si="9"/>
+        <v>1560954.2035366015</v>
+      </c>
+      <c r="H53" s="17">
+        <f t="shared" si="10"/>
+        <v>158451771.07854274</v>
+      </c>
+      <c r="I53" s="17">
+        <f t="shared" si="12"/>
+        <v>963148.2560319464</v>
+      </c>
+      <c r="J53" s="17">
+        <f t="shared" si="3"/>
+        <v>597805.94750465511</v>
+      </c>
+      <c r="K53" s="17">
+        <f t="shared" si="11"/>
+        <v>1678993.1588214231</v>
+      </c>
+      <c r="L53" s="17">
+        <f t="shared" si="4"/>
+        <v>3239947.3623580243</v>
+      </c>
+      <c r="M53" s="17">
+        <f t="shared" si="5"/>
+        <v>66422.883056072795</v>
+      </c>
+      <c r="N53" s="17">
+        <f t="shared" si="6"/>
+        <v>3173524.4793019514</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A54" s="8">
+        <v>53</v>
+      </c>
+      <c r="B54" s="17">
+        <f t="shared" si="7"/>
+        <v>156772777.91972131</v>
+      </c>
+      <c r="C54" s="9">
+        <f t="shared" si="13"/>
+        <v>0.06</v>
+      </c>
+      <c r="D54" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E54" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F54" s="11">
+        <f t="shared" si="8"/>
+        <v>0.66582238753100764</v>
+      </c>
+      <c r="G54" s="17">
+        <f t="shared" si="9"/>
+        <v>1544413.9565508333</v>
+      </c>
+      <c r="H54" s="17">
+        <f t="shared" si="10"/>
+        <v>155816261.88036942</v>
+      </c>
+      <c r="I54" s="17">
+        <f t="shared" si="12"/>
+        <v>956516.03935187845</v>
+      </c>
+      <c r="J54" s="17">
+        <f t="shared" si="3"/>
+        <v>587897.91719895485</v>
+      </c>
+      <c r="K54" s="17">
+        <f t="shared" si="11"/>
+        <v>1651066.6681067785</v>
+      </c>
+      <c r="L54" s="17">
+        <f t="shared" si="4"/>
+        <v>3195480.6246576118</v>
+      </c>
+      <c r="M54" s="17">
+        <f t="shared" si="5"/>
+        <v>65321.990799883875</v>
+      </c>
+      <c r="N54" s="17">
+        <f t="shared" si="6"/>
+        <v>3130158.633857728</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A55" s="8">
+        <v>54</v>
+      </c>
+      <c r="B55" s="17">
+        <f t="shared" si="7"/>
+        <v>154165195.21226266</v>
+      </c>
+      <c r="C55" s="9">
+        <f t="shared" si="13"/>
+        <v>0.06</v>
+      </c>
+      <c r="D55" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E55" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F55" s="11">
+        <f t="shared" si="8"/>
+        <v>0.65876717302601751</v>
+      </c>
+      <c r="G55" s="17">
+        <f t="shared" si="9"/>
+        <v>1528048.9740089101</v>
+      </c>
+      <c r="H55" s="17">
+        <f t="shared" si="10"/>
+        <v>153215265.72029972</v>
+      </c>
+      <c r="I55" s="17">
+        <f t="shared" si="12"/>
+        <v>949929.49196292518</v>
+      </c>
+      <c r="J55" s="17">
+        <f t="shared" si="3"/>
+        <v>578119.48204598494</v>
+      </c>
+      <c r="K55" s="17">
+        <f t="shared" si="11"/>
+        <v>1623505.8858627407</v>
+      </c>
+      <c r="L55" s="17">
+        <f t="shared" si="4"/>
+        <v>3151554.859871651</v>
+      </c>
+      <c r="M55" s="17">
+        <f t="shared" si="5"/>
+        <v>64235.498005109446</v>
+      </c>
+      <c r="N55" s="17">
+        <f t="shared" si="6"/>
+        <v>3087319.3618665417</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A56" s="8">
+        <v>55</v>
+      </c>
+      <c r="B56" s="17">
+        <f t="shared" si="7"/>
+        <v>151591759.83443698</v>
+      </c>
+      <c r="C56" s="9">
+        <f t="shared" si="13"/>
+        <v>0.06</v>
+      </c>
+      <c r="D56" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E56" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F56" s="11">
+        <f t="shared" si="8"/>
+        <v>0.65178671727447812</v>
+      </c>
+      <c r="G56" s="17">
+        <f t="shared" si="9"/>
+        <v>1511857.3987665398</v>
+      </c>
+      <c r="H56" s="17">
+        <f t="shared" si="10"/>
+        <v>150648371.53504959</v>
+      </c>
+      <c r="I56" s="17">
+        <f t="shared" si="12"/>
+        <v>943388.29938740109</v>
+      </c>
+      <c r="J56" s="17">
+        <f t="shared" si="3"/>
+        <v>568469.09937913867</v>
+      </c>
+      <c r="K56" s="17">
+        <f t="shared" si="11"/>
+        <v>1596306.4563636717</v>
+      </c>
+      <c r="L56" s="17">
+        <f t="shared" si="4"/>
+        <v>3108163.8551302115</v>
+      </c>
+      <c r="M56" s="17">
+        <f t="shared" si="5"/>
+        <v>63163.233264348746</v>
+      </c>
+      <c r="N56" s="17">
+        <f t="shared" si="6"/>
+        <v>3045000.6218658625</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A57" s="8">
+        <v>56</v>
+      </c>
+      <c r="B57" s="17">
+        <f t="shared" si="7"/>
+        <v>149052065.07868591</v>
+      </c>
+      <c r="C57" s="9">
+        <f t="shared" si="13"/>
+        <v>0.06</v>
+      </c>
+      <c r="D57" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E57" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F57" s="11">
+        <f t="shared" si="8"/>
+        <v>0.64488022811461843</v>
+      </c>
+      <c r="G57" s="17">
+        <f t="shared" si="9"/>
+        <v>1495837.3933581791</v>
+      </c>
+      <c r="H57" s="17">
+        <f t="shared" si="10"/>
+        <v>148115172.92937282</v>
+      </c>
+      <c r="I57" s="17">
+        <f t="shared" si="12"/>
+        <v>936892.14931310702</v>
+      </c>
+      <c r="J57" s="17">
+        <f t="shared" si="3"/>
+        <v>558945.24404507212</v>
+      </c>
+      <c r="K57" s="17">
+        <f t="shared" si="11"/>
+        <v>1569464.0733475867</v>
+      </c>
+      <c r="L57" s="17">
+        <f t="shared" si="4"/>
+        <v>3065301.4667057656</v>
+      </c>
+      <c r="M57" s="17">
+        <f t="shared" si="5"/>
+        <v>62105.027116119134</v>
+      </c>
+      <c r="N57" s="17">
+        <f t="shared" si="6"/>
+        <v>3003196.4395896466</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A58" s="8">
+        <v>57</v>
+      </c>
+      <c r="B58" s="17">
+        <f t="shared" si="7"/>
+        <v>146545708.85602522</v>
+      </c>
+      <c r="C58" s="9">
+        <f t="shared" si="13"/>
+        <v>0.06</v>
+      </c>
+      <c r="D58" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E58" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F58" s="11">
+        <f t="shared" si="8"/>
+        <v>0.63804692177860445</v>
+      </c>
+      <c r="G58" s="17">
+        <f t="shared" si="9"/>
+        <v>1479987.1397885126</v>
+      </c>
+      <c r="H58" s="17">
+        <f t="shared" si="10"/>
+        <v>145615268.12444681</v>
+      </c>
+      <c r="I58" s="17">
+        <f t="shared" si="12"/>
+        <v>930440.73157841805</v>
+      </c>
+      <c r="J58" s="17">
+        <f t="shared" si="3"/>
+        <v>549546.40821009455</v>
+      </c>
+      <c r="K58" s="17">
+        <f t="shared" si="11"/>
+        <v>1542974.4794692385</v>
+      </c>
+      <c r="L58" s="17">
+        <f t="shared" si="4"/>
+        <v>3022961.6192577509</v>
+      </c>
+      <c r="M58" s="17">
+        <f t="shared" si="5"/>
+        <v>61060.71202334384</v>
+      </c>
+      <c r="N58" s="17">
+        <f t="shared" si="6"/>
+        <v>2961900.907234407</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A59" s="8">
+        <v>58</v>
+      </c>
+      <c r="B59" s="17">
+        <f t="shared" si="7"/>
+        <v>144072293.64497757</v>
+      </c>
+      <c r="C59" s="9">
+        <f t="shared" si="13"/>
+        <v>0.06</v>
+      </c>
+      <c r="D59" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E59" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F59" s="11">
+        <f t="shared" si="8"/>
+        <v>0.63128602280359503</v>
+      </c>
+      <c r="G59" s="17">
+        <f t="shared" si="9"/>
+        <v>1464304.8393261412</v>
+      </c>
+      <c r="H59" s="17">
+        <f t="shared" si="10"/>
+        <v>143148259.90682009</v>
+      </c>
+      <c r="I59" s="17">
+        <f t="shared" si="12"/>
+        <v>924033.73815747525</v>
+      </c>
+      <c r="J59" s="17">
+        <f t="shared" si="3"/>
+        <v>540271.10116866592</v>
+      </c>
+      <c r="K59" s="17">
+        <f t="shared" si="11"/>
+        <v>1516833.4657591532</v>
+      </c>
+      <c r="L59" s="17">
+        <f t="shared" si="4"/>
+        <v>2981138.3050852944</v>
+      </c>
+      <c r="M59" s="17">
+        <f t="shared" si="5"/>
+        <v>60030.122352073988</v>
+      </c>
+      <c r="N59" s="17">
+        <f t="shared" si="6"/>
+        <v>2921108.1827332205</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A60" s="8">
+        <v>59</v>
+      </c>
+      <c r="B60" s="17">
+        <f t="shared" si="7"/>
+        <v>141631426.44106093</v>
+      </c>
+      <c r="C60" s="9">
+        <f t="shared" si="13"/>
+        <v>0.06</v>
+      </c>
+      <c r="D60" s="9">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+      <c r="E60" s="10">
+        <f t="shared" si="2"/>
+        <v>1.0596241035318976E-2</v>
+      </c>
+      <c r="F60" s="11">
+        <f t="shared" si="8"/>
+        <v>0.62459676394374031</v>
+      </c>
+      <c r="G60" s="17">
+        <f t="shared" si="9"/>
+        <v>1448788.7122994573</v>
+      </c>
+      <c r="H60" s="17">
+        <f t="shared" si="10"/>
+        <v>140713755.57791546</v>
+      </c>
+      <c r="I60" s="17">
+        <f t="shared" si="12"/>
+        <v>917670.86314547877</v>
+      </c>
+      <c r="J60" s="17">
+        <f t="shared" si="3"/>
+        <v>531117.84915397852</v>
+      </c>
+      <c r="K60" s="17">
+        <f t="shared" si="11"/>
+        <v>1491036.8710885523</v>
+      </c>
+      <c r="L60" s="17">
+        <f t="shared" si="4"/>
+        <v>2939825.5833880096</v>
+      </c>
+      <c r="M60" s="17">
+        <f t="shared" si="5"/>
+        <v>59013.09435044205</v>
+      </c>
+      <c r="N60" s="17">
+        <f t="shared" si="6"/>
+        <v>2880812.4890375677</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A61" s="8">
+        <v>60</v>
+      </c>
+      <c r="B61" s="17">
+        <f t="shared" si="7"/>
+        <v>139222718.7068269</v>
+      </c>
+      <c r="C61" s="9">
+        <v>1</v>
+      </c>
+      <c r="D61" s="9">
+        <v>1</v>
+      </c>
+      <c r="E61" s="10">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F61" s="11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G61" s="17">
+        <f t="shared" si="9"/>
+        <v>1433436.9978946829</v>
+      </c>
+      <c r="H61" s="17">
+        <f t="shared" si="10"/>
+        <v>138311366.9040828</v>
+      </c>
+      <c r="I61" s="17">
+        <f t="shared" si="12"/>
+        <v>911351.80274408206</v>
+      </c>
+      <c r="J61" s="17">
+        <f t="shared" si="3"/>
+        <v>522085.19515060086</v>
+      </c>
+      <c r="K61" s="17">
+        <f t="shared" si="11"/>
+        <v>138311366.9040828</v>
+      </c>
+      <c r="L61" s="17">
+        <f t="shared" si="4"/>
+        <v>139744803.90197748</v>
+      </c>
+      <c r="M61" s="17">
+        <f t="shared" si="5"/>
+        <v>58009.466127844542</v>
+      </c>
+      <c r="N61" s="17">
+        <f t="shared" si="6"/>
+        <v>139686794.43584964</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A62" s="8">
+        <v>61</v>
+      </c>
+      <c r="B62" s="17">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F62" s="11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G62" s="17">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H62" s="17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I62" s="17">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="J62" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K62" s="17">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="L62" s="17">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M62" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N62" s="17">
+        <f>L62-M62</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>